<commit_message>
adjust m4 uppers (slight mk12 nerf)
</commit_message>
<xml_diff>
--- a/changes/m4-uppers.xlsx
+++ b/changes/m4-uppers.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C9C14BCE-9322-4DB3-8975-0F35EF11086C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA3BAFA3-BD0C-4442-BAFE-445C9DDA937B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="m4-uppers" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -148,7 +161,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -687,9 +700,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -727,7 +740,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -833,7 +846,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -975,24 +988,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1067,7 +1080,7 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <f>C3-D3*20-E3*0.8-F3*0.6-H3*2+J3/300</f>
+        <f t="shared" ref="N3:N14" si="0">C3-D3*20-E3*0.8-F3*0.6-H3*5+J3/300</f>
         <v>-4</v>
       </c>
     </row>
@@ -1082,19 +1095,19 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="M4">
         <v>1000</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N15" si="0">C4-D4*20-E4*0.8-F4*0.6-H4*2+J4/300</f>
+        <f t="shared" si="0"/>
         <v>-2</v>
       </c>
     </row>
@@ -1136,20 +1149,20 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
       </c>
       <c r="M6">
         <v>3000</v>
       </c>
       <c r="N6">
         <f t="shared" si="0"/>
-        <v>-1.8</v>
+        <v>-1.8000000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1179,7 +1192,7 @@
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>-2.1999999999999997</v>
+        <v>-1.9</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1290,7 +1303,7 @@
       </c>
       <c r="N11">
         <f t="shared" si="0"/>
-        <v>-1.3000000000000007</v>
+        <v>-1.1500000000000008</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1301,13 +1314,13 @@
         <v>34</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F12">
         <v>-1</v>
@@ -1317,7 +1330,7 @@
       </c>
       <c r="N12">
         <f t="shared" si="0"/>
-        <v>-2.1999999999999997</v>
+        <v>-2.2000000000000006</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1358,7 +1371,7 @@
         <v>4</v>
       </c>
       <c r="D14">
-        <v>0.24</v>
+        <v>0.25</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -1377,7 +1390,7 @@
       </c>
       <c r="N14">
         <f t="shared" si="0"/>
-        <v>-1.8666666666666665</v>
+        <v>-1.7666666666666668</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1391,7 +1404,7 @@
         <v>3</v>
       </c>
       <c r="D15">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1400,17 +1413,17 @@
         <v>-1</v>
       </c>
       <c r="H15">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="J15">
-        <v>-200</v>
+        <v>-100</v>
       </c>
       <c r="M15">
         <v>2500</v>
       </c>
       <c r="N15">
-        <f t="shared" si="0"/>
-        <v>-1.7666666666666671</v>
+        <f>C15-D15*20-E15*0.8-F15*0.6-H15*5+J15/300</f>
+        <v>-1.8333333333333337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix mk12 upper again
</commit_message>
<xml_diff>
--- a/changes/m4-uppers.xlsx
+++ b/changes/m4-uppers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA3BAFA3-BD0C-4442-BAFE-445C9DDA937B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{211F10D6-2F7B-4354-A506-04C70FB8A9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -999,7 +999,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,7 +1080,7 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N14" si="0">C3-D3*20-E3*0.8-F3*0.6-H3*5+J3/300</f>
+        <f t="shared" ref="N3:N14" si="0">C3-D3*20-E3*0.8-F3*0.6-H3*5+J3/200</f>
         <v>-4</v>
       </c>
     </row>
@@ -1374,10 +1374,10 @@
         <v>0.25</v>
       </c>
       <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
         <v>2</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
       </c>
       <c r="H14">
         <v>-0.1</v>
@@ -1390,7 +1390,7 @@
       </c>
       <c r="N14">
         <f t="shared" si="0"/>
-        <v>-1.7666666666666668</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1422,8 +1422,8 @@
         <v>2500</v>
       </c>
       <c r="N15">
-        <f>C15-D15*20-E15*0.8-F15*0.6-H15*5+J15/300</f>
-        <v>-1.8333333333333337</v>
+        <f>C15-D15*20-E15*0.8-F15*0.6-H15*5+J15/200</f>
+        <v>-2.0000000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
increase mk12 price to 2000
</commit_message>
<xml_diff>
--- a/changes/m4-uppers.xlsx
+++ b/changes/m4-uppers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{211F10D6-2F7B-4354-A506-04C70FB8A9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50C045C-BF53-44D3-A05E-D747F69620D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -999,7 +999,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,7 +1386,7 @@
         <v>100</v>
       </c>
       <c r="M14">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="N14">
         <f t="shared" si="0"/>

</xml_diff>